<commit_message>
Add parametric regression results
- for exchanges
</commit_message>
<xml_diff>
--- a/analysis/results/parametric_regressions_all_market_NASDAQ.xlsx
+++ b/analysis/results/parametric_regressions_all_market_NASDAQ.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
   <si>
     <t xml:space="preserve">                       OLS Regression Results                      </t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">  Adj. R-squared:    </t>
   </si>
   <si>
-    <t xml:space="preserve">   0.481  </t>
+    <t xml:space="preserve">   0.482  </t>
   </si>
   <si>
     <t xml:space="preserve">Method:          </t>
@@ -59,16 +59,16 @@
     <t xml:space="preserve">  F-statistic:       </t>
   </si>
   <si>
-    <t>-2.411e+13</t>
+    <t>-4.255e+12</t>
   </si>
   <si>
     <t xml:space="preserve">Date:            </t>
   </si>
   <si>
-    <t>Wed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 21 Mar 2018</t>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22 Mar 2018</t>
   </si>
   <si>
     <t xml:space="preserve">  Prob (F-statistic):</t>
@@ -80,25 +80,25 @@
     <t xml:space="preserve">Time:            </t>
   </si>
   <si>
-    <t xml:space="preserve">19:57:09        </t>
+    <t xml:space="preserve">14:29:10        </t>
   </si>
   <si>
     <t xml:space="preserve">  Log-Likelihood:    </t>
   </si>
   <si>
-    <t xml:space="preserve">  248.21  </t>
+    <t xml:space="preserve">  247.49  </t>
   </si>
   <si>
     <t>No. Observations:</t>
   </si>
   <si>
-    <t xml:space="preserve">  1115          </t>
+    <t xml:space="preserve">  1114          </t>
   </si>
   <si>
     <t xml:space="preserve">  AIC:               </t>
   </si>
   <si>
-    <t xml:space="preserve">  -204.4  </t>
+    <t xml:space="preserve">  -205.0  </t>
   </si>
   <si>
     <t xml:space="preserve">Df Residuals:    </t>
@@ -110,13 +110,13 @@
     <t xml:space="preserve">  BIC:               </t>
   </si>
   <si>
-    <t xml:space="preserve">   528.0  </t>
+    <t xml:space="preserve">   522.3  </t>
   </si>
   <si>
     <t xml:space="preserve">Df Model:        </t>
   </si>
   <si>
-    <t xml:space="preserve">   145          </t>
+    <t xml:space="preserve">   144          </t>
   </si>
   <si>
     <t xml:space="preserve">                     </t>
@@ -293,13 +293,13 @@
     <t xml:space="preserve">Omnibus:      </t>
   </si>
   <si>
-    <t>460.597</t>
+    <t>459.960</t>
   </si>
   <si>
     <t xml:space="preserve">  Durbin-Watson:     </t>
   </si>
   <si>
-    <t xml:space="preserve">   1.974 </t>
+    <t xml:space="preserve">   1.898 </t>
   </si>
   <si>
     <t>Prob(Omnibus):</t>
@@ -311,13 +311,13 @@
     <t xml:space="preserve">  Jarque-Bera (JB):  </t>
   </si>
   <si>
-    <t>14221.006</t>
+    <t>14178.725</t>
   </si>
   <si>
     <t xml:space="preserve">Skew:         </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1.268 </t>
+    <t xml:space="preserve"> 1.267 </t>
   </si>
   <si>
     <t xml:space="preserve">  Prob(JB):          </t>
@@ -329,37 +329,49 @@
     <t xml:space="preserve">Kurtosis:     </t>
   </si>
   <si>
-    <t xml:space="preserve">20.311 </t>
+    <t xml:space="preserve">20.293 </t>
   </si>
   <si>
     <t xml:space="preserve">  Cond. No.          </t>
   </si>
   <si>
-    <t xml:space="preserve">1.76e+18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.542  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.475  </t>
-  </si>
-  <si>
-    <t>-1.323e+12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  239.71  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -191.4  </t>
+    <t xml:space="preserve">3.08e+18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      OLS Regression Results                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.542 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.475 </t>
+  </si>
+  <si>
+    <t>2.790e+13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:29:11        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  239.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -192.0 </t>
   </si>
   <si>
     <t xml:space="preserve">   971          </t>
   </si>
   <si>
-    <t xml:space="preserve">   531.0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   143          </t>
+    <t xml:space="preserve">   525.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   142          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
   </si>
   <si>
     <t xml:space="preserve">    0.1665</t>
@@ -443,40 +455,43 @@
     <t>-4.08e-05</t>
   </si>
   <si>
-    <t>477.676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.977 </t>
-  </si>
-  <si>
-    <t>14589.233</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.344 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.516 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.26e+18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.554  </t>
+    <t>477.017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.909 </t>
+  </si>
+  <si>
+    <t>14545.944</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.343 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.497 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.76e+18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.553  </t>
   </si>
   <si>
     <t xml:space="preserve">   0.487  </t>
   </si>
   <si>
-    <t>-1.359e+12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  253.97  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -215.9  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   516.5  </t>
+    <t>-1.714e+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:29:12        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  253.24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -216.5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   510.8  </t>
   </si>
   <si>
     <t xml:space="preserve">    0.4306</t>
@@ -599,22 +614,22 @@
     <t xml:space="preserve">    0.011</t>
   </si>
   <si>
-    <t>446.767</t>
-  </si>
-  <si>
-    <t>13424.689</t>
+    <t>446.145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.906 </t>
+  </si>
+  <si>
+    <t>13384.649</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.217 </t>
   </si>
   <si>
-    <t xml:space="preserve">19.824 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.09e+18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                      OLS Regression Results                      </t>
+    <t xml:space="preserve">19.806 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.11e+17 </t>
   </si>
   <si>
     <t xml:space="preserve">   0.544 </t>
@@ -623,22 +638,16 @@
     <t xml:space="preserve">   0.477 </t>
   </si>
   <si>
-    <t>1.145e+13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  242.04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -196.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   526.3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         </t>
+    <t>8.267e+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  241.33 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -196.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   520.6 </t>
   </si>
   <si>
     <t xml:space="preserve">    0.1370</t>
@@ -719,22 +728,22 @@
     <t xml:space="preserve">    0.012</t>
   </si>
   <si>
-    <t>463.550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.975 </t>
-  </si>
-  <si>
-    <t>13636.628</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.295 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.936 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.58e+18 </t>
+    <t>462.907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.922 </t>
+  </si>
+  <si>
+    <t>13596.023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.294 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.918 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.86e+18 </t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1503,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1511,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1525,7 +1534,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1539,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1556,7 +1565,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1564,13 +1573,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1584,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1592,13 +1601,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1606,13 +1615,13 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1626,7 +1635,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1657,68 +1666,68 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
         <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1726,13 +1735,13 @@
         <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
         <v>69</v>
@@ -1741,7 +1750,7 @@
         <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1749,22 +1758,22 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1772,13 +1781,13 @@
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1792,7 +1801,7 @@
         <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1800,7 +1809,7 @@
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
         <v>100</v>
@@ -1814,13 +1823,13 @@
         <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C20" t="s">
         <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1870,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1884,7 +1893,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1898,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1923,13 +1932,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1943,7 +1952,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1957,7 +1966,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2016,22 +2025,22 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G12" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2039,22 +2048,22 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2062,22 +2071,22 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G14" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2085,22 +2094,22 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E15" t="s">
         <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2108,68 +2117,68 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E16" t="s">
         <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G16" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G17" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E18" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" t="s">
         <v>191</v>
       </c>
-      <c r="F18" t="s">
-        <v>186</v>
-      </c>
       <c r="G18" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2177,13 +2186,13 @@
         <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2197,7 +2206,7 @@
         <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2205,7 +2214,7 @@
         <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C21" t="s">
         <v>100</v>
@@ -2219,13 +2228,13 @@
         <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C22" t="s">
         <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2258,7 +2267,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2275,7 +2284,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2289,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2303,7 +2312,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2320,7 +2329,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2328,13 +2337,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2348,7 +2357,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2356,13 +2365,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2370,13 +2379,13 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>206</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2390,7 +2399,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2421,114 +2430,114 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F12" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G12" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G13" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E14" t="s">
         <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F15" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G15" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D16" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E16" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G16" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2536,13 +2545,13 @@
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2556,7 +2565,7 @@
         <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2564,7 +2573,7 @@
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C19" t="s">
         <v>100</v>
@@ -2578,13 +2587,13 @@
         <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C20" t="s">
         <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>